<commit_message>
A small change added
</commit_message>
<xml_diff>
--- a/Week2-Assignments/Gokhan Cakal/Transformer Calculator Gokhan.xlsx
+++ b/Week2-Assignments/Gokhan Cakal/Transformer Calculator Gokhan.xlsx
@@ -94,9 +94,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>Single Phase Transofmer Design</t>
-  </si>
-  <si>
     <t>=</t>
   </si>
   <si>
@@ -380,6 +377,9 @@
   </si>
   <si>
     <t>kW</t>
+  </si>
+  <si>
+    <t>Single Phase Transformer Design</t>
   </si>
 </sst>
 </file>
@@ -1072,7 +1072,7 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -1094,7 +1094,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="26.25" customHeight="1">
       <c r="A1" s="16" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -1132,14 +1132,14 @@
     </row>
     <row r="3" spans="1:17" ht="28.5">
       <c r="A3" s="18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="20"/>
       <c r="F3" s="5"/>
       <c r="G3" s="24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H3" s="24"/>
       <c r="I3" s="24"/>
@@ -1154,27 +1154,27 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2">
         <v>34.5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H4" s="21"/>
       <c r="I4" s="21"/>
       <c r="J4" s="21"/>
       <c r="K4" s="6"/>
       <c r="L4" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M4" s="22"/>
       <c r="N4" s="22"/>
@@ -1184,66 +1184,66 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2">
         <v>0.4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I5" s="2">
         <f>ROUND(vin*C4/C5,0)</f>
         <v>1294</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K5" s="6"/>
       <c r="L5" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N5" s="11">
         <f>0.000000017*I16/(I10/1000000)</f>
         <v>3.9733080543579713</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P5" s="5"/>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2">
         <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6" s="2">
         <f>VOUT/(C5)</f>
@@ -1254,39 +1254,39 @@
       </c>
       <c r="K6" s="6"/>
       <c r="L6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N6" s="11">
         <f>0.000000017*I18/(I11/1000000)*1000</f>
         <v>0.54490907517433851</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P6" s="5"/>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2">
         <v>1000</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7" s="11">
         <f>VOUT/C4/0.98</f>
@@ -1297,218 +1297,218 @@
       </c>
       <c r="K7" s="6"/>
       <c r="L7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N7" s="11">
         <f>I7^2*N5/1000</f>
         <v>3.4758569618238879</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P7" s="5"/>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" s="2">
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I8" s="14">
         <f>C4*1000/4.44/I5/C9/C8*10000</f>
         <v>600.48456493587867</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N8" s="11">
         <f>I6^2*N6/1000/1000</f>
         <v>3.4056817198396159</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P8" s="5"/>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="2">
         <v>50</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I9" s="11">
         <f>SQRT(I8)</f>
         <v>24.504786571930772</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K9" s="6"/>
       <c r="L9" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N9" s="11">
         <f>C14*I22/1000</f>
         <v>1.5738362702613906</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P9" s="5"/>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" s="2">
         <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I10" s="11">
         <f>I7/C10</f>
         <v>7.3942620526471465</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N10" s="11">
         <f>(N8+N7+N9)</f>
         <v>8.4553749519248935</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P10" s="5"/>
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2">
         <v>0.6</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I11" s="14">
         <f>I6/C10</f>
         <v>625</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N11" s="11">
         <f>100*(VOUT*1000*pbudget)/(VOUT*1000*pbudget+N10*1000)</f>
         <v>98.954132137172351</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P11" s="5"/>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" s="2">
         <v>7750</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I12" s="14">
         <f>(I5*I10+vin*I11)/fs/100</f>
         <v>315.71958493542348</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -1519,30 +1519,30 @@
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2">
         <v>8960</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I13" s="11">
         <f>SQRT(I12)</f>
         <v>17.768499794170118</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -1553,16 +1553,16 @@
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" s="2">
         <v>2</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="6"/>
@@ -1571,7 +1571,7 @@
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
       <c r="L14" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M14" s="15"/>
       <c r="N14" s="15"/>
@@ -1580,197 +1580,197 @@
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" s="2">
         <v>0.8</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H15" s="15"/>
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
       <c r="K15" s="7"/>
       <c r="L15" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N15" s="11">
         <f>0.04*(I9+I13)/(vrdson*PI()*0.0000004*I8/10000)</f>
         <v>22408.577601399691</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P15" s="5"/>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" s="2">
         <v>1000</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I16" s="14">
         <f>4*(I9+I13/2)*I5/100</f>
         <v>1728.2165276362596</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K16" s="6"/>
       <c r="L16" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N16" s="11">
         <f>I5^2/N15</f>
         <v>74.722993569007741</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P16" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" s="2">
         <v>10</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I17" s="14">
         <f>C13*I16*I10/1000000</f>
         <v>114.49881756596339</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K17" s="6"/>
       <c r="L17" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N17" s="11">
         <f>N16*0.04</f>
         <v>2.9889197427603098</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P17" s="5"/>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2">
         <v>3</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I18" s="11">
         <f>4*(I9+I13/2)*vin/100</f>
         <v>20.033421881409502</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K18" s="6"/>
       <c r="L18" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N18" s="11">
         <f>N16+N17</f>
         <v>77.711913311768058</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P18" s="5"/>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" s="2">
         <v>3.9</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I19" s="14">
         <f>C13*I18*I11/1000000</f>
         <v>112.18716253589322</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
@@ -1782,21 +1782,21 @@
     <row r="20" spans="1:17">
       <c r="F20" s="5"/>
       <c r="G20" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I20" s="14">
         <f>I19+I17</f>
         <v>226.68598010185661</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K20" s="6"/>
       <c r="L20" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M20" s="15"/>
       <c r="N20" s="15"/>
@@ -1806,93 +1806,93 @@
     <row r="21" spans="1:17">
       <c r="F21" s="5"/>
       <c r="G21" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I21" s="13">
         <f>((I13+2*I9)^2-(I13)^2)*I9/1000000</f>
         <v>0.10153782388783165</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K21" s="6"/>
       <c r="L21" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N21" s="12">
         <f>C18*I22*dmax</f>
         <v>9206.9421810291351</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P21" s="5"/>
     </row>
     <row r="22" spans="1:17">
       <c r="F22" s="5"/>
       <c r="G22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I22" s="14">
         <f>I21*C12</f>
         <v>786.9181351306953</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K22" s="6"/>
       <c r="L22" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N22" s="12">
         <f>C17*I20*dmax</f>
         <v>8840.7532239724078</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P22" s="5"/>
     </row>
     <row r="23" spans="1:17">
       <c r="F23" s="5"/>
       <c r="G23" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I23" s="14">
         <f>I20+I22</f>
         <v>1013.604115232552</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K23" s="6"/>
       <c r="L23" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N23" s="12">
         <f>N22+N21</f>
         <v>18047.695405001541</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P23" s="5"/>
     </row>

</xml_diff>